<commit_message>
update JSON schemas to handle thumbs Fix AWS princing in benchmark XLS file
</commit_message>
<xml_diff>
--- a/benchmark/benchmark-aws-ffmpeg.xlsx
+++ b/benchmark/benchmark-aws-ffmpeg.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="121" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="211" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -757,8 +757,8 @@
   </sheetPr>
   <dimension ref="A1:P65536"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A16" view="normal" windowProtection="false" workbookViewId="0" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100">
-      <selection activeCell="K49" activeCellId="0" pane="topLeft" sqref="K49"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A25" view="normal" windowProtection="false" workbookViewId="0" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100">
+      <selection activeCell="F42" activeCellId="0" pane="topLeft" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -1131,12 +1131,12 @@
         <v>35</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.35" outlineLevel="0" r="25">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="25">
       <c r="A25" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B25" s="21" t="n">
-        <v>0.113</v>
+        <v>0.07</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>46</v>
@@ -1164,35 +1164,35 @@
       </c>
       <c r="K25" s="23" t="n">
         <f aca="false">($B25/60/60)*E25</f>
-        <v>0.0014670225</v>
+        <v>0.000908775</v>
       </c>
       <c r="L25" s="23" t="n">
         <f aca="false">($B25/60/60)*F25</f>
-        <v>0.00207530777777778</v>
+        <v>0.00128558888888889</v>
       </c>
       <c r="M25" s="23" t="n">
         <f aca="false">($B25/60/60)*G25</f>
-        <v>0.00347261555555556</v>
+        <v>0.00215117777777778</v>
       </c>
       <c r="N25" s="23" t="n">
         <f aca="false">($B25/60/60)*H25</f>
-        <v>0.00155494277777778</v>
+        <v>0.000963238888888889</v>
       </c>
       <c r="O25" s="23" t="n">
         <f aca="false">($B25/60/60)*I25</f>
-        <v>0.00189968694444444</v>
+        <v>0.00117679722222222</v>
       </c>
       <c r="P25" s="23" t="n">
         <f aca="false">($B25/60/60)*J25</f>
-        <v>0.00299189472222222</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.35" outlineLevel="0" r="26">
+        <v>0.00185338611111111</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="26">
       <c r="A26" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B26" s="21" t="n">
-        <v>0.225</v>
+        <v>0.14</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>49</v>
@@ -1220,35 +1220,35 @@
       </c>
       <c r="K26" s="23" t="n">
         <f aca="false">($B26/60/60)*E26</f>
-        <v>0.0014856875</v>
+        <v>0.000924427777777778</v>
       </c>
       <c r="L26" s="23" t="n">
         <f aca="false">($B26/60/60)*F26</f>
-        <v>0.0018323125</v>
+        <v>0.00114010555555556</v>
       </c>
       <c r="M26" s="23" t="n">
         <f aca="false">($B26/60/60)*G26</f>
-        <v>0.0030694375</v>
+        <v>0.00190987222222222</v>
       </c>
       <c r="N26" s="23" t="n">
         <f aca="false">($B26/60/60)*H26</f>
-        <v>0.001257</v>
+        <v>0.000782133333333333</v>
       </c>
       <c r="O26" s="23" t="n">
         <f aca="false">($B26/60/60)*I26</f>
-        <v>0.0016881875</v>
+        <v>0.00105042777777778</v>
       </c>
       <c r="P26" s="23" t="n">
         <f aca="false">($B26/60/60)*J26</f>
-        <v>0.002604375</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.35" outlineLevel="0" r="27">
+        <v>0.0016205</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="27">
       <c r="A27" s="4" t="s">
         <v>51</v>
       </c>
       <c r="B27" s="21" t="n">
-        <v>0.45</v>
+        <v>0.28</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>52</v>
@@ -1276,35 +1276,35 @@
       </c>
       <c r="K27" s="23" t="n">
         <f aca="false">($B27/60/60)*E27</f>
-        <v>0.001776</v>
+        <v>0.00110506666666667</v>
       </c>
       <c r="L27" s="23" t="n">
         <f aca="false">($B27/60/60)*F27</f>
-        <v>0.001985875</v>
+        <v>0.00123565555555556</v>
       </c>
       <c r="M27" s="23" t="n">
         <f aca="false">($B27/60/60)*G27</f>
-        <v>0.003255625</v>
+        <v>0.00202572222222222</v>
       </c>
       <c r="N27" s="23" t="n">
         <f aca="false">($B27/60/60)*H27</f>
-        <v>0.00137875</v>
+        <v>0.000857888888888889</v>
       </c>
       <c r="O27" s="23" t="n">
         <f aca="false">($B27/60/60)*I27</f>
-        <v>0.00182475</v>
+        <v>0.0011354</v>
       </c>
       <c r="P27" s="23" t="n">
         <f aca="false">($B27/60/60)*J27</f>
-        <v>0.0027845</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.35" outlineLevel="0" r="28">
+        <v>0.00173257777777778</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="28">
       <c r="A28" s="4" t="s">
         <v>54</v>
       </c>
       <c r="B28" s="21" t="n">
-        <v>0.9</v>
+        <v>0.56</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>55</v>
@@ -1332,27 +1332,27 @@
       </c>
       <c r="K28" s="23" t="n">
         <f aca="false">($B28/60/60)*E28</f>
-        <v>0.002696</v>
+        <v>0.00167751111111111</v>
       </c>
       <c r="L28" s="23" t="n">
         <f aca="false">($B28/60/60)*F28</f>
-        <v>0.00236975</v>
+        <v>0.00147451111111111</v>
       </c>
       <c r="M28" s="23" t="n">
         <f aca="false">($B28/60/60)*G28</f>
-        <v>0.003565</v>
+        <v>0.00221822222222222</v>
       </c>
       <c r="N28" s="23" t="n">
         <f aca="false">($B28/60/60)*H28</f>
-        <v>0.00181925</v>
+        <v>0.00113197777777778</v>
       </c>
       <c r="O28" s="23" t="n">
         <f aca="false">($B28/60/60)*I28</f>
-        <v>0.00220375</v>
+        <v>0.00137122222222222</v>
       </c>
       <c r="P28" s="23" t="n">
         <f aca="false">($B28/60/60)*J28</f>
-        <v>0.00313225</v>
+        <v>0.00194895555555556</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.7" outlineLevel="0" r="30">
@@ -1425,12 +1425,12 @@
         <v>35</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.35" outlineLevel="0" r="32">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="32">
       <c r="A32" s="4" t="s">
         <v>58</v>
       </c>
       <c r="B32" s="25" t="n">
-        <v>0.15</v>
+        <v>0.105</v>
       </c>
       <c r="C32" s="26" t="s">
         <v>59</v>
@@ -1458,35 +1458,35 @@
       </c>
       <c r="K32" s="29" t="n">
         <f aca="false">($B32/60/60)*E32</f>
-        <v>0.000903166666666667</v>
+        <v>0.000632216666666667</v>
       </c>
       <c r="L32" s="29" t="n">
         <f aca="false">($B32/60/60)*F32</f>
-        <v>0.00122108333333333</v>
+        <v>0.000854758333333333</v>
       </c>
       <c r="M32" s="29" t="n">
         <f aca="false">($B32/60/60)*G32</f>
-        <v>0.002054</v>
+        <v>0.0014378</v>
       </c>
       <c r="N32" s="29" t="n">
         <f aca="false">($B32/60/60)*H32</f>
-        <v>0.000845916666666667</v>
+        <v>0.000592141666666667</v>
       </c>
       <c r="O32" s="29" t="n">
         <f aca="false">($B32/60/60)*I32</f>
-        <v>0.001118125</v>
+        <v>0.0007826875</v>
       </c>
       <c r="P32" s="29" t="n">
         <f aca="false">($B32/60/60)*J32</f>
-        <v>0.00174645833333333</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.35" outlineLevel="0" r="33">
+        <v>0.00122252083333333</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="33">
       <c r="A33" s="4" t="s">
         <v>60</v>
       </c>
       <c r="B33" s="30" t="n">
-        <v>0.3</v>
+        <v>0.21</v>
       </c>
       <c r="C33" s="31" t="s">
         <v>61</v>
@@ -1514,35 +1514,35 @@
       </c>
       <c r="K33" s="34" t="n">
         <f aca="false">($B33/60/60)*E33</f>
-        <v>0.0008805</v>
+        <v>0.00061635</v>
       </c>
       <c r="L33" s="34" t="n">
         <f aca="false">($B33/60/60)*F33</f>
-        <v>0.00119766666666667</v>
+        <v>0.000838366666666667</v>
       </c>
       <c r="M33" s="34" t="n">
         <f aca="false">($B33/60/60)*G33</f>
-        <v>0.00195758333333333</v>
+        <v>0.00137030833333333</v>
       </c>
       <c r="N33" s="34" t="n">
         <f aca="false">($B33/60/60)*H33</f>
-        <v>0.00083</v>
+        <v>0.000581</v>
       </c>
       <c r="O33" s="34" t="n">
         <f aca="false">($B33/60/60)*I33</f>
-        <v>0.00110016666666667</v>
+        <v>0.000770116666666667</v>
       </c>
       <c r="P33" s="34" t="n">
         <f aca="false">($B33/60/60)*J33</f>
-        <v>0.00167058333333333</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.35" outlineLevel="0" r="34">
+        <v>0.00116940833333333</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="34">
       <c r="A34" s="4" t="s">
         <v>62</v>
       </c>
       <c r="B34" s="21" t="n">
-        <v>0.6</v>
+        <v>0.42</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>63</v>
@@ -1570,35 +1570,35 @@
       </c>
       <c r="K34" s="23" t="n">
         <f aca="false">($B34/60/60)*E34</f>
-        <v>0.00111466666666667</v>
+        <v>0.000780266666666667</v>
       </c>
       <c r="L34" s="23" t="n">
         <f aca="false">($B34/60/60)*F34</f>
-        <v>0.0013905</v>
+        <v>0.00097335</v>
       </c>
       <c r="M34" s="23" t="n">
         <f aca="false">($B34/60/60)*G34</f>
-        <v>0.00218183333333333</v>
+        <v>0.00152728333333333</v>
       </c>
       <c r="N34" s="23" t="n">
         <f aca="false">($B34/60/60)*H34</f>
-        <v>0.00107933333333333</v>
+        <v>0.000755533333333333</v>
       </c>
       <c r="O34" s="23" t="n">
         <f aca="false">($B34/60/60)*I34</f>
-        <v>0.001314</v>
+        <v>0.0009198</v>
       </c>
       <c r="P34" s="23" t="n">
         <f aca="false">($B34/60/60)*J34</f>
-        <v>0.00185766666666667</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.35" outlineLevel="0" r="35">
+        <v>0.00130036666666667</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="35">
       <c r="A35" s="4" t="s">
         <v>64</v>
       </c>
       <c r="B35" s="21" t="n">
-        <v>1.2</v>
+        <v>0.84</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>65</v>
@@ -1853,27 +1853,27 @@
       </c>
       <c r="H52" s="45" t="n">
         <f aca="false">(B$52/60)*$B25</f>
-        <v>14.670225</v>
+        <v>9.08775</v>
       </c>
       <c r="I52" s="45" t="n">
         <f aca="false">(C$52/60)*$B25</f>
-        <v>20.7530777777778</v>
+        <v>12.8558888888889</v>
       </c>
       <c r="J52" s="45" t="n">
         <f aca="false">(D$52/60)*$B25</f>
-        <v>34.7261555555556</v>
+        <v>21.5117777777778</v>
       </c>
       <c r="K52" s="45" t="n">
         <f aca="false">(E$52/60)*$B25</f>
-        <v>15.5494277777778</v>
+        <v>9.63238888888889</v>
       </c>
       <c r="L52" s="45" t="n">
         <f aca="false">(F$52/60)*$B25</f>
-        <v>18.9968694444444</v>
+        <v>11.7679722222222</v>
       </c>
       <c r="M52" s="45" t="n">
         <f aca="false">(G$52/60)*$B25</f>
-        <v>29.9189472222222</v>
+        <v>18.5338611111112</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="53">
@@ -1906,27 +1906,27 @@
       </c>
       <c r="H53" s="45" t="n">
         <f aca="false">(B$53/60)*$B26</f>
-        <v>14.856875</v>
+        <v>9.24427777777777</v>
       </c>
       <c r="I53" s="45" t="n">
         <f aca="false">(C$53/60)*$B26</f>
-        <v>18.323125</v>
+        <v>11.4010555555556</v>
       </c>
       <c r="J53" s="45" t="n">
         <f aca="false">(D$53/60)*$B26</f>
-        <v>30.694375</v>
+        <v>19.0987222222222</v>
       </c>
       <c r="K53" s="45" t="n">
         <f aca="false">(E$53/60)*$B26</f>
-        <v>12.57</v>
+        <v>7.82133333333333</v>
       </c>
       <c r="L53" s="45" t="n">
         <f aca="false">(F$53/60)*$B26</f>
-        <v>16.881875</v>
+        <v>10.5042777777778</v>
       </c>
       <c r="M53" s="45" t="n">
         <f aca="false">(G$53/60)*$B26</f>
-        <v>26.04375</v>
+        <v>16.205</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="54">
@@ -1959,27 +1959,27 @@
       </c>
       <c r="H54" s="45" t="n">
         <f aca="false">(B$54/60)*$B27</f>
-        <v>17.76</v>
+        <v>11.0506666666667</v>
       </c>
       <c r="I54" s="45" t="n">
         <f aca="false">(C$54/60)*$B27</f>
-        <v>19.85875</v>
+        <v>12.3565555555555</v>
       </c>
       <c r="J54" s="45" t="n">
         <f aca="false">(D$54/60)*$B27</f>
-        <v>32.55625</v>
+        <v>20.2572222222222</v>
       </c>
       <c r="K54" s="45" t="n">
         <f aca="false">(E$54/60)*$B27</f>
-        <v>13.7875</v>
+        <v>8.57888888888887</v>
       </c>
       <c r="L54" s="45" t="n">
         <f aca="false">(F$54/60)*$B27</f>
-        <v>18.2475</v>
+        <v>11.354</v>
       </c>
       <c r="M54" s="45" t="n">
         <f aca="false">(G$54/60)*$B27</f>
-        <v>27.845</v>
+        <v>17.3257777777778</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="55">
@@ -2012,27 +2012,27 @@
       </c>
       <c r="H55" s="45" t="n">
         <f aca="false">(B$55/60)*$B28</f>
-        <v>26.96</v>
+        <v>16.7751111111111</v>
       </c>
       <c r="I55" s="45" t="n">
         <f aca="false">(C$55/60)*$B28</f>
-        <v>23.6975</v>
+        <v>14.7451111111111</v>
       </c>
       <c r="J55" s="45" t="n">
         <f aca="false">(D$55/60)*$B28</f>
-        <v>35.65</v>
+        <v>22.1822222222223</v>
       </c>
       <c r="K55" s="45" t="n">
         <f aca="false">(E$55/60)*$B28</f>
-        <v>18.1925</v>
+        <v>11.3197777777777</v>
       </c>
       <c r="L55" s="45" t="n">
         <f aca="false">(F$55/60)*$B28</f>
-        <v>22.0375</v>
+        <v>13.7122222222223</v>
       </c>
       <c r="M55" s="45" t="n">
         <f aca="false">(G$55/60)*$B28</f>
-        <v>31.3225</v>
+        <v>19.4895555555556</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="7.85" outlineLevel="0" r="56">
@@ -2079,27 +2079,27 @@
       </c>
       <c r="H57" s="49" t="n">
         <f aca="false">(B$57/60)*$B32</f>
-        <v>9.03166666666666</v>
+        <v>6.32216666666667</v>
       </c>
       <c r="I57" s="49" t="n">
         <f aca="false">(C$57/60)*$B32</f>
-        <v>12.2108333333333</v>
+        <v>8.54758333333333</v>
       </c>
       <c r="J57" s="49" t="n">
         <f aca="false">(D$57/60)*$B32</f>
-        <v>20.54</v>
+        <v>14.378</v>
       </c>
       <c r="K57" s="49" t="n">
         <f aca="false">(E$57/60)*$B32</f>
-        <v>8.45916666666667</v>
+        <v>5.92141666666667</v>
       </c>
       <c r="L57" s="49" t="n">
         <f aca="false">(F$57/60)*$B32</f>
-        <v>11.18125</v>
+        <v>7.826875</v>
       </c>
       <c r="M57" s="49" t="n">
         <f aca="false">(G$57/60)*$B32</f>
-        <v>17.4645833333333</v>
+        <v>12.2252083333333</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="58">
@@ -2132,27 +2132,27 @@
       </c>
       <c r="H58" s="51" t="n">
         <f aca="false">(B$58/60)*$B33</f>
-        <v>8.805</v>
+        <v>6.1635</v>
       </c>
       <c r="I58" s="51" t="n">
         <f aca="false">(C$58/60)*$B33</f>
-        <v>11.9766666666667</v>
+        <v>8.38366666666665</v>
       </c>
       <c r="J58" s="51" t="n">
         <f aca="false">(D$58/60)*$B33</f>
-        <v>19.5758333333334</v>
+        <v>13.7030833333333</v>
       </c>
       <c r="K58" s="51" t="n">
         <f aca="false">(E$58/60)*$B33</f>
-        <v>8.3</v>
+        <v>5.81</v>
       </c>
       <c r="L58" s="51" t="n">
         <f aca="false">(F$58/60)*$B33</f>
-        <v>11.0016666666667</v>
+        <v>7.70116666666666</v>
       </c>
       <c r="M58" s="51" t="n">
         <f aca="false">(G$58/60)*$B33</f>
-        <v>16.7058333333334</v>
+        <v>11.6940833333333</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="59">
@@ -2185,27 +2185,27 @@
       </c>
       <c r="H59" s="45" t="n">
         <f aca="false">(B$59/60)*$B34</f>
-        <v>11.1466666666667</v>
+        <v>7.80266666666669</v>
       </c>
       <c r="I59" s="45" t="n">
         <f aca="false">(C$59/60)*$B34</f>
-        <v>13.905</v>
+        <v>9.7335</v>
       </c>
       <c r="J59" s="45" t="n">
         <f aca="false">(D$59/60)*$B34</f>
-        <v>21.8183333333333</v>
+        <v>15.2728333333333</v>
       </c>
       <c r="K59" s="45" t="n">
         <f aca="false">(E$59/60)*$B34</f>
-        <v>10.7933333333333</v>
+        <v>7.55533333333331</v>
       </c>
       <c r="L59" s="45" t="n">
         <f aca="false">(F$59/60)*$B34</f>
-        <v>13.14</v>
+        <v>9.198</v>
       </c>
       <c r="M59" s="45" t="n">
         <f aca="false">(G$59/60)*$B34</f>
-        <v>18.5766666666667</v>
+        <v>13.0036666666667</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="60">

</xml_diff>